<commit_message>
encounter types file updated
</commit_message>
<xml_diff>
--- a/DesignDocs/EncounterTypes.xlsx
+++ b/DesignDocs/EncounterTypes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Unity 2D\GreatGame\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0967849E-6FD2-41B9-BB64-7E809BBAAF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC2B121-AC35-44E8-BA58-C867134D8F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3930" yWindow="765" windowWidth="21600" windowHeight="11385" xr2:uid="{7F4D9BCB-BF7C-44AB-B644-D29333F29B0C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Normal</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -58,10 +58,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Soldiers dying due to diseases</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Discovering oasis</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,6 +75,26 @@
   </si>
   <si>
     <t>Oasis mirage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strong heat causing thirst - mild</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strong heat causing thirst - dangerous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Strong heat causing thirst - extremely dangerous</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low supply, Major Frankenburg in verge of death</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turcoman dying of thirst</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -103,12 +119,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -125,8 +147,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -463,16 +488,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81B743A-0A12-4EF0-B3D0-D129ADB47987}">
-  <dimension ref="B1:D5"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="41.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.3">
@@ -487,35 +513,55 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>